<commit_message>
NHSS new estimate applied
applied the new settings (province as indidivual, manually construced fixed effect terms) on the NHSS dataset; everything is OK now
</commit_message>
<xml_diff>
--- a/output/proc_1_NHSS/PCAloading_NHSS.xlsx
+++ b/output/proc_1_NHSS/PCAloading_NHSS.xlsx
@@ -14,57 +14,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve"/>
   </si>
   <si>
+    <t xml:space="preserve">RC2</t>
+  </si>
+  <si>
     <t xml:space="preserve">RC1</t>
   </si>
   <si>
+    <t xml:space="preserve">RC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medicost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permedicost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perhospitalcost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insurance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">washroom</t>
+  </si>
+  <si>
     <t xml:space="preserve">RC4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">urban</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medicost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">average</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">permedicost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">perhospitalcost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">insurance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">washroom</t>
   </si>
   <si>
     <t xml:space="preserve">distance</t>
@@ -412,231 +409,159 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.204386411137181</v>
+        <v>0.169882424467445</v>
       </c>
       <c r="C2" t="n">
-        <v>0.847646250752553</v>
+        <v>0.856508016199039</v>
       </c>
       <c r="D2" t="n">
-        <v>0.320662492345894</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-0.00177358344279719</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.126378582975825</v>
+        <v>0.224025521371875</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.522674610524168</v>
+        <v>0.77305827214502</v>
       </c>
       <c r="C3" t="n">
-        <v>0.36346966324195</v>
+        <v>0.507041796566244</v>
       </c>
       <c r="D3" t="n">
-        <v>0.569848728265632</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.373519840530374</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.12167751401524</v>
+        <v>0.165196930269257</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.505405469663388</v>
+        <v>0.862293462569513</v>
       </c>
       <c r="C4" t="n">
-        <v>0.143094734271555</v>
+        <v>0.299764367835255</v>
       </c>
       <c r="D4" t="n">
-        <v>0.649291314206546</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.402783260119787</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.118826432825688</v>
+        <v>0.174227552006935</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.371898956583464</v>
+        <v>-0.313637254321725</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.660490795268356</v>
+        <v>-0.698319723156453</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00557020758964384</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-0.372989009356556</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-0.0433680968966248</v>
+        <v>0.0610310645715462</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.870071570980206</v>
+        <v>0.543937992413105</v>
       </c>
       <c r="C6" t="n">
-        <v>0.343722248912917</v>
+        <v>0.653056618250419</v>
       </c>
       <c r="D6" t="n">
-        <v>0.20595682642504</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.103003653337095</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.0165924766408278</v>
+        <v>-0.00265297119951066</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.755094327016283</v>
+        <v>0.663445268752228</v>
       </c>
       <c r="C7" t="n">
-        <v>0.355794997079615</v>
+        <v>0.597582272238214</v>
       </c>
       <c r="D7" t="n">
-        <v>0.32315701329958</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.264307083049933</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.122718644489461</v>
+        <v>0.100020569927071</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0821158870271311</v>
+        <v>0.0881412147433429</v>
       </c>
       <c r="C8" t="n">
-        <v>0.137808322613906</v>
+        <v>0.119465228926959</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0956345810136097</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.000446691842432257</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.980503782562542</v>
+        <v>0.926353555440561</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.15732586898438</v>
+        <v>0.626760829586565</v>
       </c>
       <c r="C9" t="n">
-        <v>0.221197638916828</v>
+        <v>0.282695196552635</v>
       </c>
       <c r="D9" t="n">
-        <v>0.878011072401576</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.0864333417909864</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.0458449925804593</v>
+        <v>0.282644785792426</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.561444136316248</v>
+        <v>0.681219269474095</v>
       </c>
       <c r="C10" t="n">
-        <v>0.319802793768041</v>
+        <v>0.505110792936202</v>
       </c>
       <c r="D10" t="n">
-        <v>0.572176578104388</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.188314030702305</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.14968151168348</v>
+        <v>0.232527858890444</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.183023206136761</v>
+        <v>0.784081065692322</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0494343954375544</v>
+        <v>0.0106183988393346</v>
       </c>
       <c r="D11" t="n">
-        <v>0.203934532467289</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.91921116989376</v>
-      </c>
-      <c r="F11" t="n">
-        <v>-0.0157492080528319</v>
+        <v>-0.189056822786178</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.279575755775069</v>
+        <v>0.158881541468497</v>
       </c>
       <c r="C12" t="n">
-        <v>0.837890473209352</v>
+        <v>0.875900201029417</v>
       </c>
       <c r="D12" t="n">
-        <v>0.244269718230295</v>
-      </c>
-      <c r="E12" t="n">
-        <v>-0.00305379137284417</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.106839063788171</v>
+        <v>0.177217788458425</v>
       </c>
     </row>
   </sheetData>
@@ -658,259 +583,220 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.208718012425868</v>
+        <v>0.813994482884759</v>
       </c>
       <c r="C2" t="n">
-        <v>0.83449628924567</v>
+        <v>0.330267626518934</v>
       </c>
       <c r="D2" t="n">
-        <v>0.316953208042962</v>
+        <v>0.217264973710592</v>
       </c>
       <c r="E2" t="n">
-        <v>0.203038442073969</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-0.00230187608191894</v>
+        <v>-0.0703452882866982</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5318607311106</v>
+        <v>0.476250413049854</v>
       </c>
       <c r="C3" t="n">
-        <v>0.352338205008283</v>
+        <v>0.667259041129813</v>
       </c>
       <c r="D3" t="n">
-        <v>0.568797109180269</v>
+        <v>0.135658904081017</v>
       </c>
       <c r="E3" t="n">
-        <v>0.137689234030105</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.367255399858264</v>
+        <v>0.439704256164722</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.514405775052812</v>
+        <v>0.263283793404242</v>
       </c>
       <c r="C4" t="n">
-        <v>0.133221937737027</v>
+        <v>0.747064894265748</v>
       </c>
       <c r="D4" t="n">
-        <v>0.648800464784444</v>
+        <v>0.108279635539533</v>
       </c>
       <c r="E4" t="n">
-        <v>0.114202851069192</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.396915438710097</v>
+        <v>0.484205005749968</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.37392769524236</v>
+        <v>-0.730451991245734</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.654893300099154</v>
+        <v>-0.0573002619667246</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00888366598309062</v>
+        <v>-0.103075307748821</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.0964806773978189</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-0.375288717540807</v>
+        <v>-0.391937426523856</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.872752921603813</v>
+        <v>0.650097885940332</v>
       </c>
       <c r="C6" t="n">
-        <v>0.338885957505343</v>
+        <v>0.407625202178971</v>
       </c>
       <c r="D6" t="n">
-        <v>0.198311635348904</v>
+        <v>0.0324506775515341</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0471510278438006</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.0949220106160325</v>
+        <v>0.369833814475555</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.762332315828751</v>
+        <v>0.590074254831333</v>
       </c>
       <c r="C7" t="n">
-        <v>0.343726342974958</v>
+        <v>0.492836742886521</v>
       </c>
       <c r="D7" t="n">
-        <v>0.321142836366716</v>
+        <v>0.121872532290664</v>
       </c>
       <c r="E7" t="n">
-        <v>0.132049609239813</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.257259290507638</v>
+        <v>0.459133237049552</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0707219072596681</v>
+        <v>0.218468869595677</v>
       </c>
       <c r="C8" t="n">
-        <v>0.22189652859664</v>
+        <v>0.0655300171504124</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0531312171811185</v>
+        <v>0.928788031490058</v>
       </c>
       <c r="E8" t="n">
-        <v>0.926155779740389</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-0.00780629477003865</v>
+        <v>-0.00773907713451106</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0912013366582837</v>
+        <v>0.0766153139910086</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0616854080197</v>
+        <v>0.129154461763566</v>
       </c>
       <c r="D9" t="n">
-        <v>0.107813879036881</v>
+        <v>0.945047351701095</v>
       </c>
       <c r="E9" t="n">
-        <v>0.94619852970718</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.0146401258666962</v>
+        <v>0.0396673244247726</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>0.163925917297641</v>
+        <v>0.189799696330168</v>
       </c>
       <c r="C10" t="n">
-        <v>0.217671872833113</v>
+        <v>0.877181040801337</v>
       </c>
       <c r="D10" t="n">
-        <v>0.87587951986459</v>
+        <v>0.0678585243159713</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0632157475784242</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.0819070765325852</v>
+        <v>0.0250417384311496</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>0.568617518239062</v>
+        <v>0.45827591394823</v>
       </c>
       <c r="C11" t="n">
-        <v>0.306238632818711</v>
+        <v>0.68384233819836</v>
       </c>
       <c r="D11" t="n">
-        <v>0.569297097940965</v>
+        <v>0.162378923098814</v>
       </c>
       <c r="E11" t="n">
-        <v>0.167527746454404</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.182936246941984</v>
+        <v>0.296425790454536</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>0.19354200124417</v>
+        <v>0.0676952610292838</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0510825569124748</v>
+        <v>0.228400129491102</v>
       </c>
       <c r="D12" t="n">
-        <v>0.209194141687629</v>
+        <v>-0.0311693147171834</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.0333172704722936</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.91398905331832</v>
+        <v>0.870390581729226</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>0.289693468204666</v>
+        <v>0.847351638721142</v>
       </c>
       <c r="C13" t="n">
-        <v>0.826825209766546</v>
+        <v>0.286384153934326</v>
       </c>
       <c r="D13" t="n">
-        <v>0.248891376310809</v>
+        <v>0.146017258239216</v>
       </c>
       <c r="E13" t="n">
-        <v>0.134451202022872</v>
-      </c>
-      <c r="F13" t="n">
-        <v>-0.00989287361071033</v>
+        <v>-0.0373994749519669</v>
       </c>
     </row>
   </sheetData>
@@ -932,259 +818,220 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.208718012425868</v>
+        <v>0.813994482884759</v>
       </c>
       <c r="C2" t="n">
-        <v>0.83449628924567</v>
+        <v>0.330267626518934</v>
       </c>
       <c r="D2" t="n">
-        <v>0.316953208042962</v>
+        <v>0.217264973710592</v>
       </c>
       <c r="E2" t="n">
-        <v>0.203038442073969</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-0.00230187608191894</v>
+        <v>-0.0703452882866982</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5318607311106</v>
+        <v>0.476250413049854</v>
       </c>
       <c r="C3" t="n">
-        <v>0.352338205008283</v>
+        <v>0.667259041129813</v>
       </c>
       <c r="D3" t="n">
-        <v>0.568797109180269</v>
+        <v>0.135658904081017</v>
       </c>
       <c r="E3" t="n">
-        <v>0.137689234030105</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.367255399858264</v>
+        <v>0.439704256164722</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.514405775052812</v>
+        <v>0.263283793404242</v>
       </c>
       <c r="C4" t="n">
-        <v>0.133221937737027</v>
+        <v>0.747064894265748</v>
       </c>
       <c r="D4" t="n">
-        <v>0.648800464784444</v>
+        <v>0.108279635539533</v>
       </c>
       <c r="E4" t="n">
-        <v>0.114202851069192</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.396915438710097</v>
+        <v>0.484205005749968</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.37392769524236</v>
+        <v>-0.730451991245734</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.654893300099154</v>
+        <v>-0.0573002619667246</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00888366598309062</v>
+        <v>-0.103075307748821</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.0964806773978189</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-0.375288717540807</v>
+        <v>-0.391937426523856</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.872752921603813</v>
+        <v>0.650097885940332</v>
       </c>
       <c r="C6" t="n">
-        <v>0.338885957505343</v>
+        <v>0.407625202178971</v>
       </c>
       <c r="D6" t="n">
-        <v>0.198311635348904</v>
+        <v>0.0324506775515341</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0471510278438006</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.0949220106160325</v>
+        <v>0.369833814475555</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.762332315828751</v>
+        <v>0.590074254831333</v>
       </c>
       <c r="C7" t="n">
-        <v>0.343726342974958</v>
+        <v>0.492836742886521</v>
       </c>
       <c r="D7" t="n">
-        <v>0.321142836366716</v>
+        <v>0.121872532290664</v>
       </c>
       <c r="E7" t="n">
-        <v>0.132049609239813</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.257259290507638</v>
+        <v>0.459133237049552</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0707219072596681</v>
+        <v>0.218468869595677</v>
       </c>
       <c r="C8" t="n">
-        <v>0.22189652859664</v>
+        <v>0.0655300171504124</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0531312171811185</v>
+        <v>0.928788031490058</v>
       </c>
       <c r="E8" t="n">
-        <v>0.926155779740389</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-0.00780629477003865</v>
+        <v>-0.00773907713451106</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0912013366582837</v>
+        <v>0.0766153139910086</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0616854080197</v>
+        <v>0.129154461763566</v>
       </c>
       <c r="D9" t="n">
-        <v>0.107813879036881</v>
+        <v>0.945047351701095</v>
       </c>
       <c r="E9" t="n">
-        <v>0.94619852970718</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.0146401258666962</v>
+        <v>0.0396673244247726</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>0.163925917297641</v>
+        <v>0.189799696330168</v>
       </c>
       <c r="C10" t="n">
-        <v>0.217671872833113</v>
+        <v>0.877181040801337</v>
       </c>
       <c r="D10" t="n">
-        <v>0.87587951986459</v>
+        <v>0.0678585243159713</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0632157475784242</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.0819070765325852</v>
+        <v>0.0250417384311496</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>0.568617518239062</v>
+        <v>0.45827591394823</v>
       </c>
       <c r="C11" t="n">
-        <v>0.306238632818711</v>
+        <v>0.68384233819836</v>
       </c>
       <c r="D11" t="n">
-        <v>0.569297097940965</v>
+        <v>0.162378923098814</v>
       </c>
       <c r="E11" t="n">
-        <v>0.167527746454404</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.182936246941984</v>
+        <v>0.296425790454536</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>0.19354200124417</v>
+        <v>0.0676952610292838</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0510825569124748</v>
+        <v>0.228400129491102</v>
       </c>
       <c r="D12" t="n">
-        <v>0.209194141687629</v>
+        <v>-0.0311693147171834</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.0333172704722936</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.91398905331832</v>
+        <v>0.870390581729226</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>0.289693468204666</v>
+        <v>0.847351638721142</v>
       </c>
       <c r="C13" t="n">
-        <v>0.826825209766546</v>
+        <v>0.286384153934326</v>
       </c>
       <c r="D13" t="n">
-        <v>0.248891376310809</v>
+        <v>0.146017258239216</v>
       </c>
       <c r="E13" t="n">
-        <v>0.134451202022872</v>
-      </c>
-      <c r="F13" t="n">
-        <v>-0.00989287361071033</v>
+        <v>-0.0373994749519669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>